<commit_message>
added Butane to fluid table, adapted global variables to self.
</commit_message>
<xml_diff>
--- a/fluid_prop_VDI_Tab2.xlsx
+++ b/fluid_prop_VDI_Tab2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welp\sciebo\Carnotbatterie\Planung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welp\sciebo\Carnotbatterie\heat_transfer_prom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156358CC-3FD0-4025-91AB-A6B2F7D5E424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90928EB8-94BF-4DD6-BC88-D21BD1D0B9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1215" windowWidth="29040" windowHeight="15720" xr2:uid="{BD5AD1BA-C548-444A-823A-1120892EE797}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD5AD1BA-C548-444A-823A-1120892EE797}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -350,9 +350,6 @@
     <t>Propane</t>
   </si>
   <si>
-    <t>n-Butane</t>
-  </si>
-  <si>
     <t>n-Pentane</t>
   </si>
   <si>
@@ -393,6 +390,9 @@
   </si>
   <si>
     <t>CarbonDioxide</t>
+  </si>
+  <si>
+    <t>Butane</t>
   </si>
 </sst>
 </file>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611ECAFB-37C9-4014-90DC-179ED48D809D}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -969,7 +969,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
         <v>61</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
         <v>64</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
         <v>67</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
         <v>68</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
         <v>69</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
         <v>70</v>

</xml_diff>